<commit_message>
Added time keeping and saving student response
</commit_message>
<xml_diff>
--- a/stud_detail.xlsx
+++ b/stud_detail.xlsx
@@ -1,39 +1,58 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\BE PROJECT\Computerised-adaptive-assesments\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25D4F177-2D6E-4775-9E01-E85990A9AEE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="5">
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>roll number</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <sz val="8"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -52,12 +71,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -357,132 +385,168 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:T2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AX1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col width="11.85546875" customWidth="1" min="2" max="3"/>
+    <col min="2" max="3" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>roll number</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>q1</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>a1</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>q2</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>a2</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>q3</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>a3</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>q4</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>a4</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>q5</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>a5</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>q6</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>a6</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>q7</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>a7</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>q9</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>a9</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>q10</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>a10</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>adarsh</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>1258</v>
+    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>4</v>
+      </c>
+      <c r="R1" t="s">
+        <v>2</v>
+      </c>
+      <c r="S1" t="s">
+        <v>3</v>
+      </c>
+      <c r="T1" t="s">
+        <v>4</v>
+      </c>
+      <c r="U1" t="s">
+        <v>2</v>
+      </c>
+      <c r="V1" t="s">
+        <v>3</v>
+      </c>
+      <c r="W1" t="s">
+        <v>4</v>
+      </c>
+      <c r="X1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added some features in graph gen
</commit_message>
<xml_diff>
--- a/stud_detail.xlsx
+++ b/stud_detail.xlsx
@@ -356,10 +356,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF2"/>
+  <dimension ref="A1:AF13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
@@ -537,7 +537,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>151245</t>
+          <t>0112</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -547,58 +547,1210 @@
         <v>2</v>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>2.076088905334473</v>
       </c>
       <c r="F2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G2" t="n">
         <v>3</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>3.798868656158447</v>
       </c>
       <c r="I2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K2" t="n">
-        <v>5</v>
+        <v>2.369394302368164</v>
       </c>
       <c r="L2" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="M2" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="N2" t="n">
-        <v>2</v>
+        <v>1.285252809524536</v>
       </c>
       <c r="O2" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="P2" t="n">
         <v>3</v>
       </c>
       <c r="Q2" t="n">
-        <v>14</v>
+        <v>1.091408252716064</v>
       </c>
       <c r="R2" t="n">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="S2" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="T2" t="n">
-        <v>0</v>
+        <v>1.068862676620483</v>
       </c>
       <c r="U2" t="n">
         <v>19</v>
       </c>
       <c r="V2" t="n">
         <v>0</v>
+      </c>
+      <c r="W2" t="n">
+        <v>0.8827669620513916</v>
+      </c>
+      <c r="X2" t="n">
+        <v>22</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>0.7628440856933594</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>23</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>0.643791675567627</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>26</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>0.4999361038208008</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>adarsh 2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>22121</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>4.445470571517944</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" t="n">
+        <v>2.931854248046875</v>
+      </c>
+      <c r="I3" t="n">
+        <v>4</v>
+      </c>
+      <c r="J3" t="n">
+        <v>2</v>
+      </c>
+      <c r="K3" t="n">
+        <v>3.948999881744385</v>
+      </c>
+      <c r="L3" t="n">
+        <v>11</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="n">
+        <v>2.417903423309326</v>
+      </c>
+      <c r="O3" t="n">
+        <v>13</v>
+      </c>
+      <c r="P3" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>1.360247373580933</v>
+      </c>
+      <c r="R3" t="n">
+        <v>14</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0</v>
+      </c>
+      <c r="T3" t="n">
+        <v>4.245097637176514</v>
+      </c>
+      <c r="U3" t="n">
+        <v>15</v>
+      </c>
+      <c r="V3" t="n">
+        <v>2</v>
+      </c>
+      <c r="W3" t="n">
+        <v>2.63466477394104</v>
+      </c>
+      <c r="X3" t="n">
+        <v>18</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>3.889636039733887</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>19</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>7.052731990814209</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>22</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>1.651203632354736</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>adarsh 3</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>5555</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1.64252495765686</v>
+      </c>
+      <c r="F4" t="n">
+        <v>2</v>
+      </c>
+      <c r="G4" t="n">
+        <v>3</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1.145309448242188</v>
+      </c>
+      <c r="I4" t="n">
+        <v>3</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.3531234264373779</v>
+      </c>
+      <c r="L4" t="n">
+        <v>4</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.3227417469024658</v>
+      </c>
+      <c r="O4" t="n">
+        <v>5</v>
+      </c>
+      <c r="P4" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0.7523236274719238</v>
+      </c>
+      <c r="R4" t="n">
+        <v>7</v>
+      </c>
+      <c r="S4" t="n">
+        <v>2</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0.5193734169006348</v>
+      </c>
+      <c r="U4" t="n">
+        <v>11</v>
+      </c>
+      <c r="V4" t="n">
+        <v>3</v>
+      </c>
+      <c r="W4" t="n">
+        <v>0.4801175594329834</v>
+      </c>
+      <c r="X4" t="n">
+        <v>14</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>1.843168497085571</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>18</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>1.154319047927856</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>19</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>2.228299140930176</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>ashdv</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>5487</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>2</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1.052364826202393</v>
+      </c>
+      <c r="F5" t="n">
+        <v>2</v>
+      </c>
+      <c r="G5" t="n">
+        <v>3</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.3253095149993896</v>
+      </c>
+      <c r="I5" t="n">
+        <v>3</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.3109369277954102</v>
+      </c>
+      <c r="L5" t="n">
+        <v>4</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.393150806427002</v>
+      </c>
+      <c r="O5" t="n">
+        <v>5</v>
+      </c>
+      <c r="P5" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0.3068628311157227</v>
+      </c>
+      <c r="R5" t="n">
+        <v>7</v>
+      </c>
+      <c r="S5" t="n">
+        <v>2</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0.291844367980957</v>
+      </c>
+      <c r="U5" t="n">
+        <v>11</v>
+      </c>
+      <c r="V5" t="n">
+        <v>3</v>
+      </c>
+      <c r="W5" t="n">
+        <v>0.2683188915252686</v>
+      </c>
+      <c r="X5" t="n">
+        <v>14</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>2.417190074920654</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>15</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>2</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>0.4644284248352051</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>18</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>0.9979376792907715</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>ajsdh</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>8452</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>3.157140016555786</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.768733024597168</v>
+      </c>
+      <c r="I6" t="n">
+        <v>5</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>1.809016466140747</v>
+      </c>
+      <c r="L6" t="n">
+        <v>6</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="n">
+        <v>1.58581018447876</v>
+      </c>
+      <c r="O6" t="n">
+        <v>9</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>2.114368915557861</v>
+      </c>
+      <c r="R6" t="n">
+        <v>12</v>
+      </c>
+      <c r="S6" t="n">
+        <v>1</v>
+      </c>
+      <c r="T6" t="n">
+        <v>1.456769466400146</v>
+      </c>
+      <c r="U6" t="n">
+        <v>13</v>
+      </c>
+      <c r="V6" t="n">
+        <v>2</v>
+      </c>
+      <c r="W6" t="n">
+        <v>1.625339508056641</v>
+      </c>
+      <c r="X6" t="n">
+        <v>14</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>1.920741558074951</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>18</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>1.713698863983154</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>1.407757043838501</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>asdsa</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>5845</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>2</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1.481217622756958</v>
+      </c>
+      <c r="F7" t="n">
+        <v>2</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.6238429546356201</v>
+      </c>
+      <c r="I7" t="n">
+        <v>4</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.4460091590881348</v>
+      </c>
+      <c r="L7" t="n">
+        <v>5</v>
+      </c>
+      <c r="M7" t="n">
+        <v>1</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.4591681957244873</v>
+      </c>
+      <c r="O7" t="n">
+        <v>7</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0.5594687461853027</v>
+      </c>
+      <c r="R7" t="n">
+        <v>9</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0.5117449760437012</v>
+      </c>
+      <c r="U7" t="n">
+        <v>12</v>
+      </c>
+      <c r="V7" t="n">
+        <v>0</v>
+      </c>
+      <c r="W7" t="n">
+        <v>0.4960389137268066</v>
+      </c>
+      <c r="X7" t="n">
+        <v>16</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>0.9158885478973389</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>22</v>
+      </c>
+      <c r="AB7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC7" t="n">
+        <v>0.4833309650421143</v>
+      </c>
+      <c r="AD7" t="n">
+        <v>23</v>
+      </c>
+      <c r="AE7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF7" t="n">
+        <v>1.209952592849731</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>aslads</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>23435</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>2</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1.700097799301147</v>
+      </c>
+      <c r="F8" t="n">
+        <v>2</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>5.674262046813965</v>
+      </c>
+      <c r="I8" t="n">
+        <v>4</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>1.891043663024902</v>
+      </c>
+      <c r="L8" t="n">
+        <v>5</v>
+      </c>
+      <c r="M8" t="n">
+        <v>1</v>
+      </c>
+      <c r="N8" t="n">
+        <v>2.98143458366394</v>
+      </c>
+      <c r="O8" t="n">
+        <v>7</v>
+      </c>
+      <c r="P8" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>1.651224136352539</v>
+      </c>
+      <c r="R8" t="n">
+        <v>11</v>
+      </c>
+      <c r="S8" t="n">
+        <v>0</v>
+      </c>
+      <c r="T8" t="n">
+        <v>1.6232750415802</v>
+      </c>
+      <c r="U8" t="n">
+        <v>13</v>
+      </c>
+      <c r="V8" t="n">
+        <v>0</v>
+      </c>
+      <c r="W8" t="n">
+        <v>1.934630155563354</v>
+      </c>
+      <c r="X8" t="n">
+        <v>16</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>1.939390897750854</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>17</v>
+      </c>
+      <c r="AB8" t="n">
+        <v>2</v>
+      </c>
+      <c r="AC8" t="n">
+        <v>1.607932806015015</v>
+      </c>
+      <c r="AD8" t="n">
+        <v>18</v>
+      </c>
+      <c r="AE8" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF8" t="n">
+        <v>1.937278032302856</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>aspdfksda</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>15444</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>2</v>
+      </c>
+      <c r="E9" t="n">
+        <v>3.405494689941406</v>
+      </c>
+      <c r="F9" t="n">
+        <v>2</v>
+      </c>
+      <c r="G9" t="n">
+        <v>3</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.6916184425354004</v>
+      </c>
+      <c r="I9" t="n">
+        <v>3</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>1.084953546524048</v>
+      </c>
+      <c r="L9" t="n">
+        <v>4</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" t="n">
+        <v>2.435461044311523</v>
+      </c>
+      <c r="O9" t="n">
+        <v>5</v>
+      </c>
+      <c r="P9" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>0.5269999504089355</v>
+      </c>
+      <c r="R9" t="n">
+        <v>7</v>
+      </c>
+      <c r="S9" t="n">
+        <v>0</v>
+      </c>
+      <c r="T9" t="n">
+        <v>1.713361978530884</v>
+      </c>
+      <c r="U9" t="n">
+        <v>9</v>
+      </c>
+      <c r="V9" t="n">
+        <v>1</v>
+      </c>
+      <c r="W9" t="n">
+        <v>1.098459959030151</v>
+      </c>
+      <c r="X9" t="n">
+        <v>10</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>1.226040124893188</v>
+      </c>
+      <c r="AA9" t="n">
+        <v>12</v>
+      </c>
+      <c r="AB9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC9" t="n">
+        <v>0.8307409286499023</v>
+      </c>
+      <c r="AD9" t="n">
+        <v>16</v>
+      </c>
+      <c r="AE9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF9" t="n">
+        <v>1.171280384063721</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>asdh</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>15245</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>2.245107650756836</v>
+      </c>
+      <c r="F10" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" t="n">
+        <v>1.32030200958252</v>
+      </c>
+      <c r="I10" t="n">
+        <v>4</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.6662743091583252</v>
+      </c>
+      <c r="L10" t="n">
+        <v>5</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0.9925205707550049</v>
+      </c>
+      <c r="O10" t="n">
+        <v>6</v>
+      </c>
+      <c r="P10" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>2.235407590866089</v>
+      </c>
+      <c r="R10" t="n">
+        <v>7</v>
+      </c>
+      <c r="S10" t="n">
+        <v>0</v>
+      </c>
+      <c r="T10" t="n">
+        <v>2.96513295173645</v>
+      </c>
+      <c r="U10" t="n">
+        <v>9</v>
+      </c>
+      <c r="V10" t="n">
+        <v>0</v>
+      </c>
+      <c r="W10" t="n">
+        <v>0.6910746097564697</v>
+      </c>
+      <c r="X10" t="n">
+        <v>12</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z10" t="n">
+        <v>1.563397407531738</v>
+      </c>
+      <c r="AA10" t="n">
+        <v>13</v>
+      </c>
+      <c r="AB10" t="n">
+        <v>2</v>
+      </c>
+      <c r="AC10" t="n">
+        <v>1.093145847320557</v>
+      </c>
+      <c r="AD10" t="n">
+        <v>14</v>
+      </c>
+      <c r="AE10" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF10" t="n">
+        <v>2.516886711120605</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>askdashd</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>454154</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E11" t="n">
+        <v>3.477753639221191</v>
+      </c>
+      <c r="F11" t="n">
+        <v>2</v>
+      </c>
+      <c r="G11" t="n">
+        <v>3</v>
+      </c>
+      <c r="H11" t="n">
+        <v>5.968281030654907</v>
+      </c>
+      <c r="I11" t="n">
+        <v>3</v>
+      </c>
+      <c r="J11" t="n">
+        <v>3</v>
+      </c>
+      <c r="K11" t="n">
+        <v>1.257969617843628</v>
+      </c>
+      <c r="L11" t="n">
+        <v>11</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0.7327044010162354</v>
+      </c>
+      <c r="O11" t="n">
+        <v>13</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>0.8621106147766113</v>
+      </c>
+      <c r="R11" t="n">
+        <v>16</v>
+      </c>
+      <c r="S11" t="n">
+        <v>0</v>
+      </c>
+      <c r="T11" t="n">
+        <v>0.5233442783355713</v>
+      </c>
+      <c r="U11" t="n">
+        <v>22</v>
+      </c>
+      <c r="V11" t="n">
+        <v>0</v>
+      </c>
+      <c r="W11" t="n">
+        <v>1.139888286590576</v>
+      </c>
+      <c r="X11" t="n">
+        <v>23</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>1.203319549560547</v>
+      </c>
+      <c r="AA11" t="n">
+        <v>26</v>
+      </c>
+      <c r="AB11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC11" t="n">
+        <v>1.561362981796265</v>
+      </c>
+      <c r="AD11" t="n">
+        <v>30</v>
+      </c>
+      <c r="AE11" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF11" t="n">
+        <v>2.215673923492432</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>sdjfn</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>5457712</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>2</v>
+      </c>
+      <c r="E12" t="n">
+        <v>2.082211256027222</v>
+      </c>
+      <c r="F12" t="n">
+        <v>2</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>1.391033887863159</v>
+      </c>
+      <c r="I12" t="n">
+        <v>4</v>
+      </c>
+      <c r="J12" t="n">
+        <v>2</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.467536449432373</v>
+      </c>
+      <c r="L12" t="n">
+        <v>11</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0.5028867721557617</v>
+      </c>
+      <c r="O12" t="n">
+        <v>13</v>
+      </c>
+      <c r="P12" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>0.454653263092041</v>
+      </c>
+      <c r="R12" t="n">
+        <v>14</v>
+      </c>
+      <c r="S12" t="n">
+        <v>0</v>
+      </c>
+      <c r="T12" t="n">
+        <v>2.031610488891602</v>
+      </c>
+      <c r="U12" t="n">
+        <v>15</v>
+      </c>
+      <c r="V12" t="n">
+        <v>0</v>
+      </c>
+      <c r="W12" t="n">
+        <v>0.4424777030944824</v>
+      </c>
+      <c r="X12" t="n">
+        <v>16</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>0.6108808517456055</v>
+      </c>
+      <c r="AA12" t="n">
+        <v>17</v>
+      </c>
+      <c r="AB12" t="n">
+        <v>2</v>
+      </c>
+      <c r="AC12" t="n">
+        <v>1.011982440948486</v>
+      </c>
+      <c r="AD12" t="n">
+        <v>18</v>
+      </c>
+      <c r="AE12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF12" t="n">
+        <v>1.08799147605896</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>sdfhsdf</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>46451</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" t="n">
+        <v>4.292492151260376</v>
+      </c>
+      <c r="F13" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.8461611270904541</v>
+      </c>
+      <c r="I13" t="n">
+        <v>5</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.319453239440918</v>
+      </c>
+      <c r="L13" t="n">
+        <v>6</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0.2467446327209473</v>
+      </c>
+      <c r="O13" t="n">
+        <v>9</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>1.648900032043457</v>
+      </c>
+      <c r="R13" t="n">
+        <v>12</v>
+      </c>
+      <c r="S13" t="n">
+        <v>0</v>
+      </c>
+      <c r="T13" t="n">
+        <v>0.5291614532470703</v>
+      </c>
+      <c r="U13" t="n">
+        <v>16</v>
+      </c>
+      <c r="V13" t="n">
+        <v>0</v>
+      </c>
+      <c r="W13" t="n">
+        <v>1.435649633407593</v>
+      </c>
+      <c r="X13" t="n">
+        <v>22</v>
+      </c>
+      <c r="Y13" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>0.84759521484375</v>
+      </c>
+      <c r="AA13" t="n">
+        <v>23</v>
+      </c>
+      <c r="AB13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC13" t="n">
+        <v>2.764688491821289</v>
+      </c>
+      <c r="AD13" t="n">
+        <v>26</v>
+      </c>
+      <c r="AE13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF13" t="n">
+        <v>0.7866451740264893</v>
       </c>
     </row>
   </sheetData>

</xml_diff>